<commit_message>
Mejora README y actualización Excel
</commit_message>
<xml_diff>
--- a/Planes de operación_tenologias.xlsx
+++ b/Planes de operación_tenologias.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://idom-my.sharepoint.com/personal/mateo_rodriguez_idom_com/Documents/Escritorio/Tecnologia_buses/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="209" documentId="8_{0A57E7E6-CDA8-401A-BBD9-8E5F970D2806}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{E493C7D1-3F07-4496-8B66-08061E17C517}"/>
+  <xr:revisionPtr revIDLastSave="216" documentId="8_{0A57E7E6-CDA8-401A-BBD9-8E5F970D2806}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1BB50C82-AE51-4CA1-BAFD-30C69045CD96}"/>
   <bookViews>
     <workbookView xWindow="-25305" yWindow="-4185" windowWidth="12810" windowHeight="15135" firstSheet="2" activeTab="3" xr2:uid="{3C259509-320D-4E0F-80E6-50C4AA9A57C0}"/>
   </bookViews>
@@ -1680,13 +1680,14 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9:B11"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="23.42578125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="13.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -1759,6 +1760,9 @@
       <c r="A8" t="s">
         <v>86</v>
       </c>
+      <c r="C8">
+        <v>21</v>
+      </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
@@ -1771,6 +1775,10 @@
         <f>'Carga Nocturna'!B17*360</f>
         <v>1639440</v>
       </c>
+      <c r="D9" s="3">
+        <f>B9*(C9*C8)</f>
+        <v>6541365.5999999996</v>
+      </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
@@ -1783,6 +1791,10 @@
         <f>'Carga Nocturna'!B17*360</f>
         <v>1639440</v>
       </c>
+      <c r="D10" s="3">
+        <f t="shared" ref="D10:D11" si="1">B10*(C10*C9)</f>
+        <v>1048227770304</v>
+      </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
@@ -1794,6 +1806,10 @@
       <c r="C11" s="3">
         <f>'Carga Nocturna'!B17*360</f>
         <v>1639440</v>
+      </c>
+      <c r="D11" s="3">
+        <f t="shared" si="1"/>
+        <v>430042162176</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update Planes de operación_tecnologias.xlsx
</commit_message>
<xml_diff>
--- a/Planes de operación_tenologias.xlsx
+++ b/Planes de operación_tenologias.xlsx
@@ -8,18 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://idom-my.sharepoint.com/personal/mateo_rodriguez_idom_com/Documents/Escritorio/Tecnologia_buses/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="216" documentId="8_{0A57E7E6-CDA8-401A-BBD9-8E5F970D2806}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1BB50C82-AE51-4CA1-BAFD-30C69045CD96}"/>
+  <xr:revisionPtr revIDLastSave="264" documentId="8_{0A57E7E6-CDA8-401A-BBD9-8E5F970D2806}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DFD5E59C-3413-4E45-882B-C6A10CEEF497}"/>
   <bookViews>
-    <workbookView xWindow="-25305" yWindow="-4185" windowWidth="12810" windowHeight="15135" firstSheet="2" activeTab="3" xr2:uid="{3C259509-320D-4E0F-80E6-50C4AA9A57C0}"/>
+    <workbookView minimized="1" xWindow="-26535" yWindow="-1725" windowWidth="15375" windowHeight="7785" activeTab="5" xr2:uid="{3C259509-320D-4E0F-80E6-50C4AA9A57C0}"/>
   </bookViews>
   <sheets>
     <sheet name="Resumen" sheetId="9" r:id="rId1"/>
-    <sheet name="Diesel" sheetId="1" r:id="rId2"/>
-    <sheet name="Carga Nocturna" sheetId="2" r:id="rId3"/>
-    <sheet name="$_carga_noctura" sheetId="10" r:id="rId4"/>
-    <sheet name="Carga Flash" sheetId="7" r:id="rId5"/>
-    <sheet name="Carga por oportunidad" sheetId="8" r:id="rId6"/>
-    <sheet name="Hidrogeno en cochera" sheetId="4" r:id="rId7"/>
+    <sheet name="$_carga_Diesel" sheetId="11" r:id="rId2"/>
+    <sheet name="$_carga_noctura" sheetId="10" r:id="rId3"/>
+    <sheet name="Diesel" sheetId="1" r:id="rId4"/>
+    <sheet name="Carga Nocturna" sheetId="2" r:id="rId5"/>
+    <sheet name="Carga Flash" sheetId="7" r:id="rId6"/>
+    <sheet name="Carga por oportunidad" sheetId="8" r:id="rId7"/>
+    <sheet name="Hidrogeno en cochera" sheetId="4" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="283" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="93">
   <si>
     <t>Km</t>
   </si>
@@ -312,6 +313,15 @@
   </si>
   <si>
     <t>Batería</t>
+  </si>
+  <si>
+    <t>TOTAL</t>
+  </si>
+  <si>
+    <t>Km año por bus</t>
+  </si>
+  <si>
+    <t>Tecnologia - Diesel</t>
   </si>
 </sst>
 </file>
@@ -408,7 +418,7 @@
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -440,6 +450,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Millares" xfId="1" builtinId="3"/>
@@ -860,7 +871,7 @@
   <dimension ref="A2:L12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -991,7 +1002,7 @@
       </c>
       <c r="B5" s="19">
         <f>Diesel!H7</f>
-        <v>455.40000000000003</v>
+        <v>2003.76</v>
       </c>
       <c r="C5" s="20" t="s">
         <v>73</v>
@@ -1110,11 +1121,332 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B6E1A90B-19AC-4298-B280-E626065AEDAA}">
+  <dimension ref="A1:D12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="27" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="B1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>79</v>
+      </c>
+      <c r="B4" s="3">
+        <v>150000</v>
+      </c>
+      <c r="C4">
+        <f>Resumen!B4</f>
+        <v>8</v>
+      </c>
+      <c r="D4" s="10">
+        <f>B4*C4</f>
+        <v>1200000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>80</v>
+      </c>
+      <c r="B5" s="3">
+        <v>30000</v>
+      </c>
+      <c r="C5">
+        <v>0</v>
+      </c>
+      <c r="D5" s="10">
+        <f t="shared" ref="D5:D6" si="0">B5*C5</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>81</v>
+      </c>
+      <c r="B6" s="3">
+        <v>105000</v>
+      </c>
+      <c r="C6">
+        <v>0</v>
+      </c>
+      <c r="D6" s="10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C7" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="D7" s="29">
+        <f>SUM(D4:D6)</f>
+        <v>1200000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>86</v>
+      </c>
+      <c r="C8" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>87</v>
+      </c>
+      <c r="B9" s="28">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="C9" s="3">
+        <f>('Carga Nocturna'!$B$17*246)+(('Carga Nocturna'!$B$17*0.8)*52)+(('Carga Nocturna'!$B$17*0.6)*52)</f>
+        <v>1451815.2</v>
+      </c>
+      <c r="D9" s="3">
+        <f>B9*(C9*$C$4)</f>
+        <v>6736422.527999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>88</v>
+      </c>
+      <c r="B10" s="28">
+        <v>0.39</v>
+      </c>
+      <c r="C10" s="3">
+        <f>('Carga Nocturna'!$B$17*246)+(('Carga Nocturna'!$B$17*0.8)*52)+(('Carga Nocturna'!$B$17*0.6)*52)</f>
+        <v>1451815.2</v>
+      </c>
+      <c r="D10" s="3">
+        <f t="shared" ref="D10:D11" si="1">B10*(C10*$C$4)</f>
+        <v>4529663.4239999996</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>89</v>
+      </c>
+      <c r="B11" s="28">
+        <v>0.16</v>
+      </c>
+      <c r="C11" s="3">
+        <f>('Carga Nocturna'!$B$17*246)+(('Carga Nocturna'!$B$17*0.8)*52)+(('Carga Nocturna'!$B$17*0.6)*52)</f>
+        <v>1451815.2</v>
+      </c>
+      <c r="D11" s="3">
+        <f t="shared" si="1"/>
+        <v>1858323.456</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C12" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="D12" s="29">
+        <f>SUM(D9:D11)</f>
+        <v>13124409.408</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{595B49EF-3334-40E9-928F-C29FE1065930}">
+  <dimension ref="A1:D12"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="27" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="6" t="s">
+        <v>85</v>
+      </c>
+      <c r="B1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D1" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>79</v>
+      </c>
+      <c r="B4" s="3">
+        <v>550000</v>
+      </c>
+      <c r="C4">
+        <f>'Carga Nocturna'!B21</f>
+        <v>21</v>
+      </c>
+      <c r="D4" s="10">
+        <f>B4*C4</f>
+        <v>11550000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>80</v>
+      </c>
+      <c r="B5" s="3">
+        <v>30000</v>
+      </c>
+      <c r="C5">
+        <f>'Carga Nocturna'!H12</f>
+        <v>8</v>
+      </c>
+      <c r="D5" s="10">
+        <f t="shared" ref="D5:D6" si="0">B5*C5</f>
+        <v>240000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>81</v>
+      </c>
+      <c r="B6" s="3">
+        <v>105000</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6" s="10">
+        <f t="shared" si="0"/>
+        <v>105000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C7" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="D7" s="29">
+        <f>SUM(D4:D6)</f>
+        <v>11895000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>86</v>
+      </c>
+      <c r="C8" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>87</v>
+      </c>
+      <c r="B9" s="28">
+        <v>0.19</v>
+      </c>
+      <c r="C9" s="3">
+        <f>('Carga Nocturna'!$B$17*246)+(('Carga Nocturna'!$B$17*0.8)*52)+(('Carga Nocturna'!$B$17*0.6)*52)</f>
+        <v>1451815.2</v>
+      </c>
+      <c r="D9" s="3">
+        <f>B9*(C9*$C$4)</f>
+        <v>5792742.648</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>88</v>
+      </c>
+      <c r="B10" s="28">
+        <v>0.39</v>
+      </c>
+      <c r="C10" s="3">
+        <f>('Carga Nocturna'!$B$17*246)+(('Carga Nocturna'!$B$17*0.8)*52)+(('Carga Nocturna'!$B$17*0.6)*52)</f>
+        <v>1451815.2</v>
+      </c>
+      <c r="D10" s="3">
+        <f t="shared" ref="D10:D11" si="1">B10*(C10*$C$4)</f>
+        <v>11890366.488</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>89</v>
+      </c>
+      <c r="B11" s="28">
+        <v>0.16</v>
+      </c>
+      <c r="C11" s="3">
+        <f>('Carga Nocturna'!$B$17*246)+(('Carga Nocturna'!$B$17*0.8)*52)+(('Carga Nocturna'!$B$17*0.6)*52)</f>
+        <v>1451815.2</v>
+      </c>
+      <c r="D11" s="3">
+        <f t="shared" si="1"/>
+        <v>4878099.0719999997</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C12" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="D12" s="29">
+        <f>SUM(D9:D11)</f>
+        <v>22561208.208000001</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{911EF546-0916-4E40-B4D6-352F902C78AB}">
   <dimension ref="A1:I21"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1148,8 +1480,8 @@
         <v>58</v>
       </c>
       <c r="H2">
-        <f>10/100</f>
-        <v>0.1</v>
+        <f>44/100</f>
+        <v>0.44</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
@@ -1204,7 +1536,7 @@
       </c>
       <c r="H5" s="16">
         <f>H4*H2</f>
-        <v>56.925000000000004</v>
+        <v>250.47</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -1240,7 +1572,7 @@
       </c>
       <c r="H7" s="15">
         <f>H5*B16</f>
-        <v>455.40000000000003</v>
+        <v>2003.76</v>
       </c>
       <c r="I7" t="s">
         <v>59</v>
@@ -1365,12 +1697,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C8CA0CC2-BA5B-4DE0-A0D8-32CD07E6A240}">
-  <dimension ref="A1:I21"/>
+  <dimension ref="A1:I22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B18" sqref="B18"/>
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1658,6 +1990,12 @@
       <c r="B21" s="8">
         <f>ROUNDUP(B20/B8,0)</f>
         <v>21</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B22">
+        <f>B20/B21</f>
+        <v>227.7</v>
       </c>
     </row>
   </sheetData>
@@ -1675,154 +2013,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{595B49EF-3334-40E9-928F-C29FE1065930}">
-  <dimension ref="A1:D11"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="13.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.42578125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>85</v>
-      </c>
-      <c r="B1" t="s">
-        <v>84</v>
-      </c>
-      <c r="C1" t="s">
-        <v>83</v>
-      </c>
-      <c r="D1" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>79</v>
-      </c>
-      <c r="B4" s="3">
-        <v>550000</v>
-      </c>
-      <c r="C4">
-        <f>'Carga Nocturna'!B21</f>
-        <v>21</v>
-      </c>
-      <c r="D4" s="10">
-        <f>B4*C4</f>
-        <v>11550000</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>80</v>
-      </c>
-      <c r="B5" s="3">
-        <v>30000</v>
-      </c>
-      <c r="C5">
-        <f>'Carga Nocturna'!H12</f>
-        <v>8</v>
-      </c>
-      <c r="D5" s="10">
-        <f t="shared" ref="D5:D6" si="0">B5*C5</f>
-        <v>240000</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>81</v>
-      </c>
-      <c r="B6" s="3">
-        <v>105000</v>
-      </c>
-      <c r="C6">
-        <v>1</v>
-      </c>
-      <c r="D6" s="10">
-        <f t="shared" si="0"/>
-        <v>105000</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>86</v>
-      </c>
-      <c r="C8">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>87</v>
-      </c>
-      <c r="B9" s="28">
-        <v>0.19</v>
-      </c>
-      <c r="C9" s="3">
-        <f>'Carga Nocturna'!B17*360</f>
-        <v>1639440</v>
-      </c>
-      <c r="D9" s="3">
-        <f>B9*(C9*C8)</f>
-        <v>6541365.5999999996</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>88</v>
-      </c>
-      <c r="B10" s="28">
-        <v>0.39</v>
-      </c>
-      <c r="C10" s="3">
-        <f>'Carga Nocturna'!B17*360</f>
-        <v>1639440</v>
-      </c>
-      <c r="D10" s="3">
-        <f t="shared" ref="D10:D11" si="1">B10*(C10*C9)</f>
-        <v>1048227770304</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>89</v>
-      </c>
-      <c r="B11" s="28">
-        <v>0.16</v>
-      </c>
-      <c r="C11" s="3">
-        <f>'Carga Nocturna'!B17*360</f>
-        <v>1639440</v>
-      </c>
-      <c r="D11" s="3">
-        <f t="shared" si="1"/>
-        <v>430042162176</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C97BE8C7-2021-4FD8-A404-B13B08117290}">
   <dimension ref="A1:I35"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D21" sqref="D21:E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2102,7 +2298,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>12</v>
       </c>
@@ -2114,7 +2310,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>11</v>
       </c>
@@ -2126,8 +2322,8 @@
         <v>6</v>
       </c>
     </row>
-    <row r="19" spans="1:3" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" ht="14.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>25</v>
       </c>
@@ -2135,8 +2331,12 @@
         <f>ROUNDUP(B6/B18,0)</f>
         <v>9</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D20">
+        <f>B6/B5</f>
+        <v>99</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>35</v>
       </c>
@@ -2147,8 +2347,10 @@
       <c r="C21" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D21" s="3"/>
+      <c r="E21" s="10"/>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>72</v>
       </c>
@@ -2157,7 +2359,7 @@
         <v>5382</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>36</v>
       </c>
@@ -2169,7 +2371,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>37</v>
       </c>
@@ -2178,7 +2380,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="6" t="s">
         <v>14</v>
       </c>
@@ -2187,22 +2389,22 @@
         <v>13</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B27" s="2"/>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B28" s="2"/>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B29" s="2"/>
     </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B30" s="3"/>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B31" s="3"/>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="6"/>
       <c r="B32" s="6"/>
     </row>
@@ -2221,7 +2423,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1840755F-3209-4AD3-AA8D-4005579D73A5}">
   <dimension ref="A1:I34"/>
   <sheetViews>
@@ -2629,7 +2831,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D6729C48-1F61-440A-AC7B-9BC4CEF3797C}">
   <dimension ref="A1:H20"/>
   <sheetViews>

</xml_diff>